<commit_message>
final jeopardy and typos
</commit_message>
<xml_diff>
--- a/old questions/geopardy2024.xlsx
+++ b/old questions/geopardy2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmerson\Documents\Git\geopardy\old questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB6ED98-A829-4054-8BE3-D5709633869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A185103-1059-4017-834A-C45A529A1CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="159">
   <si>
     <t>double-jeopardy</t>
   </si>
@@ -43,12 +43,6 @@
     <t>final-jeopardy</t>
   </si>
   <si>
-    <t>The Danube: Vienna, Bratislava, Budapest, and Belgrade</t>
-  </si>
-  <si>
-    <t>RIVERS &amp; CAPITALS</t>
-  </si>
-  <si>
     <t>Four European capital cities are located on this river</t>
   </si>
   <si>
@@ -436,16 +430,10 @@
     <t>What is Bălți?</t>
   </si>
   <si>
-    <t>Called teqwu?be? (pronounced Tacoma), meaning mother of waters, in Lushootseed</t>
-  </si>
-  <si>
     <t>Called Pahto by the Yakima people</t>
   </si>
   <si>
     <t>Called Lawetla'la or Loowit, meaning one from whom smoke comes, by the Cowlitz people</t>
-  </si>
-  <si>
-    <t>Although many sources indicate that Wy'est is this peak's indigenious name, the name appears to be completely fictional.</t>
   </si>
   <si>
     <t>What is Mt. Rainier?</t>
@@ -514,12 +502,27 @@
       <t xml:space="preserve">, George Meany perpetuated an erronious 1895 claim that the Duwamish called this mountain range "Sun-a-do." </t>
     </r>
   </si>
+  <si>
+    <t>Called təqʷuʔmə (pronounced Tacoma), meaning mother of waters, in Lushootseed</t>
+  </si>
+  <si>
+    <t>Although many sources indicate that Wy'est is this peak's indigenous name, the name appears to be completely fictional.</t>
+  </si>
+  <si>
+    <t>Dennis's favorite whiskey, Woodford Reserve, is from this state, which happens to have more miles of running water than any other state except Alaska.</t>
+  </si>
+  <si>
+    <t>NAME THIS STATE</t>
+  </si>
+  <si>
+    <t>What is Kentucky</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -552,6 +555,12 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -753,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -783,6 +792,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,8 +1098,8 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1097,7 +1107,7 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.54296875" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="49.54296875" customWidth="1"/>
     <col min="6" max="6" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.81640625" customWidth="1"/>
@@ -1108,25 +1118,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1134,14 +1144,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
@@ -1152,11 +1162,11 @@
       <c r="A3" s="10"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>2</v>
@@ -1167,11 +1177,11 @@
       <c r="A4" s="10"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>3</v>
@@ -1182,11 +1192,11 @@
       <c r="A5" s="10"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>4</v>
@@ -1197,11 +1207,11 @@
       <c r="A6" s="10"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>5</v>
@@ -1211,14 +1221,14 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>1</v>
@@ -1229,11 +1239,11 @@
       <c r="A8" s="10"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>2</v>
@@ -1244,11 +1254,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>3</v>
@@ -1259,11 +1269,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>4</v>
@@ -1274,11 +1284,11 @@
       <c r="A11" s="10"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>5</v>
@@ -1288,14 +1298,14 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>1</v>
@@ -1306,11 +1316,11 @@
       <c r="A13" s="10"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>2</v>
@@ -1321,11 +1331,11 @@
       <c r="A14" s="10"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>3</v>
@@ -1338,11 +1348,11 @@
       <c r="A15" s="10"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>4</v>
@@ -1353,11 +1363,11 @@
       <c r="A16" s="10"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>5</v>
@@ -1367,14 +1377,14 @@
     <row r="17" spans="1:7" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>1</v>
@@ -1385,11 +1395,11 @@
       <c r="A18" s="10"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>2</v>
@@ -1400,11 +1410,11 @@
       <c r="A19" s="10"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>3</v>
@@ -1415,11 +1425,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>4</v>
@@ -1430,11 +1440,11 @@
       <c r="A21" s="10"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>5</v>
@@ -1444,14 +1454,14 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>1</v>
@@ -1462,11 +1472,11 @@
       <c r="A23" s="10"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>2</v>
@@ -1477,11 +1487,11 @@
       <c r="A24" s="10"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>3</v>
@@ -1492,11 +1502,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>4</v>
@@ -1507,11 +1517,11 @@
       <c r="A26" s="10"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>5</v>
@@ -1521,16 +1531,16 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>1</v>
@@ -1541,13 +1551,13 @@
       <c r="A28" s="10"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>2</v>
@@ -1558,13 +1568,13 @@
       <c r="A29" s="10"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>3</v>
@@ -1575,13 +1585,13 @@
       <c r="A30" s="10"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>4</v>
@@ -1592,13 +1602,13 @@
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>5</v>
@@ -1607,20 +1617,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G32" s="6"/>
     </row>
@@ -1628,11 +1638,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>1</v>
@@ -1643,14 +1653,14 @@
       <c r="A34" s="10"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1658,11 +1668,11 @@
       <c r="A35" s="10"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>2</v>
@@ -1673,31 +1683,31 @@
       <c r="A36" s="10"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1705,11 +1715,11 @@
       <c r="A38" s="10"/>
       <c r="B38" s="12"/>
       <c r="C38" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>1</v>
@@ -1720,14 +1730,14 @@
       <c r="A39" s="10"/>
       <c r="B39" s="12"/>
       <c r="C39" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1735,11 +1745,11 @@
       <c r="A40" s="10"/>
       <c r="B40" s="12"/>
       <c r="C40" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>2</v>
@@ -1750,31 +1760,31 @@
       <c r="A41" s="10"/>
       <c r="B41" s="12"/>
       <c r="C41" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="10"/>
       <c r="B42" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1782,11 +1792,11 @@
       <c r="A43" s="10"/>
       <c r="B43" s="12"/>
       <c r="C43" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>1</v>
@@ -1797,14 +1807,14 @@
       <c r="A44" s="10"/>
       <c r="B44" s="12"/>
       <c r="C44" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1812,11 +1822,11 @@
       <c r="A45" s="10"/>
       <c r="B45" s="12"/>
       <c r="C45" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>2</v>
@@ -1827,31 +1837,31 @@
       <c r="A46" s="10"/>
       <c r="B46" s="12"/>
       <c r="C46" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="10"/>
       <c r="B47" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="18" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1859,11 +1869,11 @@
       <c r="A48" s="10"/>
       <c r="B48" s="12"/>
       <c r="C48" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>1</v>
@@ -1874,14 +1884,14 @@
       <c r="A49" s="10"/>
       <c r="B49" s="12"/>
       <c r="C49" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -1889,11 +1899,11 @@
       <c r="A50" s="10"/>
       <c r="B50" s="12"/>
       <c r="C50" s="18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="18" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>2</v>
@@ -1904,31 +1914,31 @@
       <c r="A51" s="10"/>
       <c r="B51" s="12"/>
       <c r="C51" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="18" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -1936,10 +1946,10 @@
       <c r="A53" s="10"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12" t="s">
@@ -1951,14 +1961,14 @@
       <c r="A54" s="10"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -1966,10 +1976,10 @@
       <c r="A55" s="10"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
@@ -1981,31 +1991,31 @@
       <c r="A56" s="10"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="10"/>
       <c r="B57" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -2013,11 +2023,11 @@
       <c r="A58" s="10"/>
       <c r="B58" s="12"/>
       <c r="C58" s="18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>1</v>
@@ -2028,14 +2038,14 @@
       <c r="A59" s="10"/>
       <c r="B59" s="12"/>
       <c r="C59" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2043,11 +2053,11 @@
       <c r="A60" s="10"/>
       <c r="B60" s="12"/>
       <c r="C60" s="18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>2</v>
@@ -2060,14 +2070,14 @@
       <c r="A61" s="10"/>
       <c r="B61" s="12"/>
       <c r="C61" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -2076,15 +2086,17 @@
         <v>6</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
     </row>

</xml_diff>